<commit_message>
Lisätty pistetiedot valintatapajonon exceliin
</commit_message>
<xml_diff>
--- a/src/test/resources/valintatapajono/valintatapajono.xlsx
+++ b/src/test/resources/valintatapajono/valintatapajono.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jussija\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessika/dev/oph/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/valintatapajono/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Valintatapajono" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="115">
   <si>
     <t/>
   </si>
@@ -358,6 +363,12 @@
   </si>
   <si>
     <t>sd</t>
+  </si>
+  <si>
+    <t>Kokonaispisteet</t>
+  </si>
+  <si>
+    <t>47.6</t>
   </si>
 </sst>
 </file>
@@ -398,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -408,6 +419,7 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -472,9 +484,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -507,9 +519,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -689,43 +701,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" hidden="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" hidden="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="4" customWidth="1"/>
+    <col min="6" max="8" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -739,16 +755,19 @@
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -761,8 +780,8 @@
       <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>0</v>
+      <c r="E5" s="3">
+        <v>50</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>0</v>
@@ -770,8 +789,11 @@
       <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -784,8 +806,8 @@
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>0</v>
+      <c r="E6" s="3">
+        <v>49</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>0</v>
@@ -793,8 +815,11 @@
       <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -808,7 +833,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>0</v>
@@ -816,8 +841,11 @@
       <c r="G7" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -830,8 +858,8 @@
       <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>0</v>
+      <c r="E8" s="3">
+        <v>44</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>0</v>
@@ -839,8 +867,11 @@
       <c r="G8" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -853,8 +884,8 @@
       <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>0</v>
+      <c r="E9" s="3">
+        <v>44</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>0</v>
@@ -862,8 +893,11 @@
       <c r="G9" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -876,17 +910,20 @@
       <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="3">
+        <v>43</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -897,17 +934,18 @@
       <c r="D11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -918,17 +956,18 @@
       <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -939,17 +978,18 @@
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -962,8 +1002,8 @@
       <c r="D14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>0</v>
+      <c r="E14" s="3">
+        <v>41</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>0</v>
@@ -971,8 +1011,11 @@
       <c r="G14" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -985,8 +1028,8 @@
       <c r="D15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>0</v>
+      <c r="E15" s="3">
+        <v>39</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>0</v>
@@ -994,8 +1037,11 @@
       <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -1006,17 +1052,18 @@
       <c r="D16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -1027,17 +1074,18 @@
       <c r="D17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
@@ -1048,17 +1096,18 @@
       <c r="D18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
@@ -1069,17 +1118,18 @@
       <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -1090,17 +1140,18 @@
       <c r="D20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -1111,17 +1162,18 @@
       <c r="D21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
@@ -1132,17 +1184,18 @@
       <c r="D22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
@@ -1153,17 +1206,18 @@
       <c r="D23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
@@ -1174,17 +1228,18 @@
       <c r="D24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
@@ -1195,17 +1250,18 @@
       <c r="D25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
@@ -1216,17 +1272,18 @@
       <c r="D26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>62</v>
       </c>
@@ -1237,17 +1294,18 @@
       <c r="D27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
@@ -1258,17 +1316,18 @@
       <c r="D28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
@@ -1279,17 +1338,18 @@
       <c r="D29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>68</v>
       </c>
@@ -1300,17 +1360,18 @@
       <c r="D30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
@@ -1321,17 +1382,18 @@
       <c r="D31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -1342,17 +1404,18 @@
       <c r="D32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
@@ -1363,17 +1426,18 @@
       <c r="D33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
@@ -1384,17 +1448,18 @@
       <c r="D34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>78</v>
       </c>
@@ -1405,17 +1470,18 @@
       <c r="D35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
@@ -1426,17 +1492,18 @@
       <c r="D36" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>82</v>
       </c>
@@ -1447,17 +1514,18 @@
       <c r="D37" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>84</v>
       </c>
@@ -1468,17 +1536,18 @@
       <c r="D38" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>86</v>
       </c>
@@ -1489,17 +1558,18 @@
       <c r="D39" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E39" s="3"/>
       <c r="F39" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
@@ -1510,17 +1580,18 @@
       <c r="D40" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
@@ -1531,17 +1602,18 @@
       <c r="D41" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>92</v>
       </c>
@@ -1552,17 +1624,18 @@
       <c r="D42" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>94</v>
       </c>
@@ -1573,17 +1646,18 @@
       <c r="D43" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E43" s="3"/>
       <c r="F43" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>96</v>
       </c>
@@ -1594,17 +1668,18 @@
       <c r="D44" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E44" s="3"/>
       <c r="F44" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>98</v>
       </c>
@@ -1615,17 +1690,18 @@
       <c r="D45" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>100</v>
       </c>
@@ -1636,17 +1712,18 @@
       <c r="D46" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>102</v>
       </c>
@@ -1657,17 +1734,18 @@
       <c r="D47" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>104</v>
       </c>
@@ -1678,17 +1756,18 @@
       <c r="D48" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>106</v>
       </c>
@@ -1699,17 +1778,18 @@
       <c r="D49" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E49" s="3"/>
       <c r="F49" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>108</v>
       </c>
@@ -1720,346 +1800,32 @@
       <c r="D50" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E50" s="3"/>
       <c r="F50" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="H50" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1"/>
   <mergeCells count="2">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
-  <dataValidations count="92">
-    <dataValidation type="decimal" allowBlank="1" sqref="B5">
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" sqref="B5:B50">
       <formula1>0</formula1>
       <formula2>46</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D5">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B6">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D6">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B7">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D7">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B8">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D8">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B9">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D9">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B10">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D10">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B11">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D11">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B12">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D12">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B13">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D13">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B14">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D14">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B15">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D15">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B16">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D16">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B17">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D17">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B18">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D18">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B19">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D19">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B20">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D20">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B21">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D21">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B22">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D22">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B23">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D23">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B24">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D24">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B25">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D25">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B26">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D26">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B27">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D27">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B28">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D28">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B29">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D29">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B30">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D30">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B31">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D31">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B32">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D32">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B33">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D33">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B34">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D34">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B35">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D35">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B36">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D36">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B37">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D37">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B38">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D38">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B39">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D39">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B40">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D40">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B41">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D41">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B42">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D42">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B43">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D43">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B44">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D44">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B45">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D45">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B46">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D46">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B47">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D47">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B48">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D48">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B49">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D49">
-      <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" sqref="B50">
-      <formula1>0</formula1>
-      <formula2>46</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D50">
+    <dataValidation type="list" allowBlank="1" sqref="D5:E50">
       <formula1>"Määrittelemätön,Hyväksyttävissä,Hylätty"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>